<commit_message>
Updated some of data with 1bn instruction runs.
</commit_message>
<xml_diff>
--- a/figs_src/data2.xlsx
+++ b/figs_src/data2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6165" yWindow="3660" windowWidth="19035" windowHeight="13035" activeTab="4"/>
+    <workbookView xWindow="6165" yWindow="3660" windowWidth="19035" windowHeight="13035"/>
   </bookViews>
   <sheets>
     <sheet name="exec_time" sheetId="1" r:id="rId1"/>
@@ -190,13 +190,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-4.8825939827284379E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-4.1276786536529941E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-4.9205946397415504E-2</c:v>
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -248,13 +245,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.0510290830846428E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-3.9029076598610657E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.1637502315329005E-4</c:v>
+                  <c:v>3.09E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -306,13 +300,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-4.7286768640103352E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-7.0406999587914465E-5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.5407754172749198E-2</c:v>
+                  <c:v>-1.6899999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -364,245 +355,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-2.3724374080053793E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.1171950847536827E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.9618113510002101E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>exec_time!$F$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>400%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>exec_time!$A$4:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>unrestricted dropping</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>source dropping</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sub-flow dropping</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>exec_time!$F$4:$F$6</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2.9936249912911786E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-6.8566216950888964E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-3.666964163962666E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>exec_time!$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>500%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>exec_time!$A$4:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>unrestricted dropping</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>source dropping</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sub-flow dropping</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>exec_time!$G$4:$G$6</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>-2.7141582006760437E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2202703094475305E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.8507695487018014E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>exec_time!$H$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>600%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>exec_time!$A$4:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>unrestricted dropping</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>source dropping</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sub-flow dropping</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>exec_time!$H$4:$H$6</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>-2.8730631512815089E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.1755752916737379E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.688550855192511E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>exec_time!$I$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>700% overhead</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>exec_time!$A$4:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>unrestricted dropping</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>source dropping</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sub-flow dropping</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>exec_time!$I$4:$I$6</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>-1.4994021339565899E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.2453859182962517E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-3.1933929815530483E-2</c:v>
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -617,11 +373,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108288256"/>
-        <c:axId val="108335872"/>
+        <c:axId val="150828160"/>
+        <c:axId val="150829696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108288256"/>
+        <c:axId val="150828160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,7 +386,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="108335872"/>
+        <c:crossAx val="150829696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -638,7 +394,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108335872"/>
+        <c:axId val="150829696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,13 +417,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108288256"/>
+        <c:crossAx val="150828160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -779,13 +536,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-2.71755179382181E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.8497949860364559E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.4383168132213515E-2</c:v>
+                  <c:v>1.15E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1900000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -837,13 +591,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.1997333138719672E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.555455807545854E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.4665127758158549E-3</c:v>
+                  <c:v>5.7000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4999999999999997E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -895,13 +646,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.4485789845529441E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.5960224316204719E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.6473540111327996E-2</c:v>
+                  <c:v>-9.2999999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.5000000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -953,245 +701,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-4.6367482215069269E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.5640142187790634E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.810577778301126E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>exec_time!$F$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>400%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>exec_time!$A$10:$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>unrestricted dropping</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>source dropping</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sub-flow dropping</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>exec_time!$F$10:$F$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>-1.9985488771027612E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.5164242779245925E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.6637779183190911E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>exec_time!$G$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>500%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>exec_time!$A$10:$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>unrestricted dropping</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>source dropping</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sub-flow dropping</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>exec_time!$G$10:$G$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.9668717219726073E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.1088344712280926E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7235516866612441E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>exec_time!$H$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>600%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>exec_time!$A$10:$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>unrestricted dropping</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>source dropping</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sub-flow dropping</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>exec_time!$H$10:$H$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>-4.5414312408456406E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.9780279618591846E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.4455397905028722E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>exec_time!$I$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>700% overhead</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>exec_time!$A$10:$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>unrestricted dropping</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>source dropping</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sub-flow dropping</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>exec_time!$I$10:$I$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>4.4024407646194877E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.4125946086895934E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-5.8877191508716342E-3</c:v>
+                  <c:v>-2.5600000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9.2999999999999992E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1206,11 +719,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="108700416"/>
-        <c:axId val="108701952"/>
+        <c:axId val="150909696"/>
+        <c:axId val="150911232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108700416"/>
+        <c:axId val="150909696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1219,7 +732,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="108701952"/>
+        <c:crossAx val="150911232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1227,7 +740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108701952"/>
+        <c:axId val="150911232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,13 +763,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108700416"/>
+        <c:crossAx val="150909696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1368,13 +882,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.8455120563184462E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.9763973626997563</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.46170470293988164</c:v>
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1426,13 +937,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.22020573192476001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.48241214922897058</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.70889437964035884</c:v>
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1484,13 +992,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.64099322958865368</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.26330792958451499</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.68312029236202598</c:v>
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1542,13 +1047,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.8267915299793711E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.76628786472226773</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.28054510077767991</c:v>
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1600,13 +1102,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.32455541731343251</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.74231894512715724</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.90709484739337054</c:v>
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1658,13 +1157,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.9877040874671792E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.34509133415322768</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.64790578215205497</c:v>
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1716,13 +1212,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.637073826253225E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.24165319085911519</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.12369706386866408</c:v>
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1774,13 +1267,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.44579406928491283</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.57019675265981229</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.85538041836008349</c:v>
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1795,11 +1285,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="131130112"/>
-        <c:axId val="131131648"/>
+        <c:axId val="151015808"/>
+        <c:axId val="151017344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="131130112"/>
+        <c:axId val="151015808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,7 +1298,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131131648"/>
+        <c:crossAx val="151017344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1816,7 +1306,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131131648"/>
+        <c:axId val="151017344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1840,13 +1330,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131130112"/>
+        <c:crossAx val="151015808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1958,13 +1449,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.45731313139805163</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.25477908235141589</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.9577819134638561</c:v>
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2016,13 +1504,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.6802512612172732</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.35271894149669181</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.97285605678552922</c:v>
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2074,13 +1559,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.38806738845137323</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.39097989231502039</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.4491679749822034</c:v>
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2132,13 +1614,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.48949685213912608</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.95515654458441424</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.8515800413183916</c:v>
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2190,13 +1669,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.78309723496215899</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.55354569495583994</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.24371279947253677</c:v>
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2248,13 +1724,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.85689814435531697</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.10883217263780842</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.54412292972641974</c:v>
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2306,13 +1779,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.16096299682713944</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.52441433405000271</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.29289412003016757</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2364,13 +1834,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.89734917584782481</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.21233707388446565</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15488918266240836</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2385,11 +1852,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142746752"/>
-        <c:axId val="142748288"/>
+        <c:axId val="151228416"/>
+        <c:axId val="151229952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142746752"/>
+        <c:axId val="151228416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2398,7 +1865,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142748288"/>
+        <c:crossAx val="151229952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2406,7 +1873,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142748288"/>
+        <c:axId val="151229952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2437,7 +1904,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142746752"/>
+        <c:crossAx val="151228416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2485,7 +1952,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="224" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="346" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2497,7 +1964,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="224" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="346" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2509,7 +1976,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="224" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="346" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2521,7 +1988,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="224" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="346" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2533,7 +2000,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="3082868" cy="2181395"/>
+    <xdr:ext cx="2929075" cy="2026127"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2560,7 +2027,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="3082868" cy="2181395"/>
+    <xdr:ext cx="2929075" cy="2026127"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2587,7 +2054,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="3082868" cy="2181395"/>
+    <xdr:ext cx="2929075" cy="2026127"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2614,7 +2081,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="3082868" cy="2181395"/>
+    <xdr:ext cx="2929075" cy="2026127"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4034,8 +3501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4084,36 +3551,28 @@
         <v>0</v>
       </c>
       <c r="B4" s="2">
-        <f ca="1">RAND()/10-0.05</f>
-        <v>-4.8825939827284379E-3</v>
+        <v>0.04</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:I6" ca="1" si="0">RAND()/10-0.05</f>
-        <v>6.0510290830846428E-3</v>
+        <v>3.09E-2</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-4.7286768640103352E-2</v>
+        <v>-1.6899999999999998E-2</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-2.3724374080053793E-2</v>
+        <v>0.09</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.9936249912911786E-2</v>
+        <v>-0.35010000000000002</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-2.7141582006760437E-2</v>
+        <v>-0.51939999999999997</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-2.8730631512815089E-2</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-1.4994021339565899E-2</v>
+        <v>0.1275</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -4121,74 +3580,42 @@
         <v>1</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" ref="B5:B6" ca="1" si="1">RAND()/10-0.05</f>
-        <v>-4.1276786536529941E-2</v>
+        <v>15.14</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-3.9029076598610657E-2</v>
+        <v>14.64</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-7.0406999587914465E-5</v>
+        <v>13.64</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.1171950847536827E-2</v>
+        <v>12.64</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-6.8566216950888964E-3</v>
+        <v>11.64</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.2202703094475305E-2</v>
+        <v>10.65</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.1755752916737379E-2</v>
+        <v>9.65</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.2453859182962517E-2</v>
+        <v>8.65</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>-4.9205946397415504E-2</v>
-      </c>
-      <c r="C6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.1637502315329005E-4</v>
-      </c>
-      <c r="D6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.5407754172749198E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.9618113510002101E-2</v>
-      </c>
-      <c r="F6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-3.666964163962666E-2</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.8507695487018014E-3</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.688550855192511E-2</v>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>-3.1933929815530483E-2</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -4226,36 +3653,28 @@
         <v>0</v>
       </c>
       <c r="B10" s="2">
-        <f ca="1">RAND()/10-0.05</f>
-        <v>-2.71755179382181E-2</v>
+        <v>1.15E-2</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" ref="C10:I12" ca="1" si="2">RAND()/10-0.05</f>
-        <v>4.1997333138719672E-3</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>3.4485789845529441E-2</v>
+        <v>-9.2999999999999992E-3</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>-4.6367482215069269E-2</v>
+        <v>-2.5600000000000001E-2</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>-1.9985488771027612E-3</v>
+        <v>-0.43559999999999999</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.9668717219726073E-2</v>
+        <v>-0.62360000000000004</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>-4.5414312408456406E-2</v>
+        <v>-1.1329</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.4024407646194877E-2</v>
+        <v>-2.0855999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -4263,74 +3682,42 @@
         <v>1</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" ref="B11:B12" ca="1" si="3">RAND()/10-0.05</f>
-        <v>-2.8497949860364559E-2</v>
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>9.555455807545854E-4</v>
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>-2.5960224316204719E-3</v>
+        <v>-2.5000000000000001E-3</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.5640142187790634E-3</v>
+        <v>-9.2999999999999992E-3</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.5164242779245925E-2</v>
+        <v>-0.58350000000000002</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>7.1088344712280926E-3</v>
+        <v>-1.5834999999999999</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>3.9780279618591846E-3</v>
+        <v>-2.5834999999999999</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.4125946086895934E-2</v>
+        <v>-3.5834999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.4383168132213515E-2</v>
-      </c>
-      <c r="C12" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.4665127758158549E-3</v>
-      </c>
-      <c r="D12" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.6473540111327996E-2</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>3.810577778301126E-2</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.6637779183190911E-2</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.7235516866612441E-2</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>2.4455397905028722E-2</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>-5.8877191508716342E-3</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -4373,36 +3760,28 @@
         <v>0</v>
       </c>
       <c r="B17" s="1">
-        <f ca="1">RAND()</f>
-        <v>4.8455120563184462E-3</v>
+        <v>0.88</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" ref="C17:I19" ca="1" si="4">RAND()</f>
-        <v>0.22020573192476001</v>
+        <v>0.89</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.64099322958865368</v>
+        <v>0.91</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>7.8267915299793711E-2</v>
+        <v>0.92</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.32455541731343251</v>
+        <v>0.93</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>1.9877040874671792E-2</v>
+        <v>0.94</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>5.637073826253225E-2</v>
+        <v>0.96</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.44579406928491283</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -4410,74 +3789,42 @@
         <v>1</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" ref="B18:B19" ca="1" si="5">RAND()</f>
-        <v>0.9763973626997563</v>
+        <v>0.94</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.48241214922897058</v>
+        <v>0.94</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.26330792958451499</v>
+        <v>0.96</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.76628786472226773</v>
+        <v>0.96</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.74231894512715724</v>
+        <v>0.97</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.34509133415322768</v>
+        <v>0.97</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.24165319085911519</v>
+        <v>0.98</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.57019675265981229</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="1">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.46170470293988164</v>
-      </c>
-      <c r="C19" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.70889437964035884</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.68312029236202598</v>
-      </c>
-      <c r="E19" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.28054510077767991</v>
-      </c>
-      <c r="F19" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.90709484739337054</v>
-      </c>
-      <c r="G19" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.64790578215205497</v>
-      </c>
-      <c r="H19" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.12369706386866408</v>
-      </c>
-      <c r="I19" s="1">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.85538041836008349</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -4515,36 +3862,28 @@
         <v>0</v>
       </c>
       <c r="B23" s="1">
-        <f ca="1">RAND()</f>
-        <v>0.45731313139805163</v>
+        <v>0.49</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" ref="C23:I25" ca="1" si="6">RAND()</f>
-        <v>0.6802512612172732</v>
+        <v>0.63</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.38806738845137323</v>
+        <v>0.82</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.48949685213912608</v>
+        <v>0.95</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.78309723496215899</v>
+        <v>0.98</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.85689814435531697</v>
+        <v>0.99</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.16096299682713944</v>
+        <v>1</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.89734917584782481</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -4552,74 +3891,42 @@
         <v>1</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" ref="B24:B25" ca="1" si="7">RAND()</f>
-        <v>0.25477908235141589</v>
+        <v>0.52</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.35271894149669181</v>
+        <v>0.67</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.39097989231502039</v>
+        <v>0.88</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.95515654458441424</v>
+        <v>0.99</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.55354569495583994</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.10883217263780842</v>
+        <v>1</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.52441433405000271</v>
+        <v>1</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.21233707388446565</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="1">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.9577819134638561</v>
-      </c>
-      <c r="C25" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.97285605678552922</v>
-      </c>
-      <c r="D25" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.4491679749822034</v>
-      </c>
-      <c r="E25" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.8515800413183916</v>
-      </c>
-      <c r="F25" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.24371279947253677</v>
-      </c>
-      <c r="G25" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.54412292972641974</v>
-      </c>
-      <c r="H25" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.29289412003016757</v>
-      </c>
-      <c r="I25" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.15488918266240836</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added data for comparing policies.
</commit_message>
<xml_diff>
--- a/figs_src/data2.xlsx
+++ b/figs_src/data2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6165" yWindow="3660" windowWidth="19035" windowHeight="13035" activeTab="6"/>
+    <workbookView xWindow="6165" yWindow="3660" windowWidth="19035" windowHeight="13035" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="exec_time" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,12 @@
     <sheet name="umc_coverage" sheetId="8" r:id="rId5"/>
     <sheet name="prob_1m_20140324" sheetId="2" r:id="rId6"/>
     <sheet name="prob_1m" sheetId="9" r:id="rId7"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId8"/>
+    <sheet name="bc_policies" sheetId="3" r:id="rId8"/>
+    <sheet name="bc_policy_coverage" sheetId="12" r:id="rId9"/>
+    <sheet name="bc_policy_exec_time" sheetId="11" r:id="rId10"/>
+    <sheet name="umc_policies" sheetId="10" r:id="rId11"/>
+    <sheet name="umc_policy_exec_time" sheetId="14" r:id="rId12"/>
+    <sheet name="umc_policy_coverage" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="42">
   <si>
     <t>unrestricted dropping</t>
   </si>
@@ -111,11 +116,56 @@
   <si>
     <t xml:space="preserve">6 runs </t>
   </si>
+  <si>
+    <t>perlbench</t>
+  </si>
+  <si>
+    <t>bzip2</t>
+  </si>
+  <si>
+    <t>gcc</t>
+  </si>
+  <si>
+    <t>mcf</t>
+  </si>
+  <si>
+    <t>gobmk</t>
+  </si>
+  <si>
+    <t>hmmer</t>
+  </si>
+  <si>
+    <t>sjeng</t>
+  </si>
+  <si>
+    <t>libquantum</t>
+  </si>
+  <si>
+    <t>h264ref</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>Unrestricted Dropping</t>
+  </si>
+  <si>
+    <t>Source-Only Dropping</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,10 +213,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -434,11 +485,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="150873984"/>
-        <c:axId val="150875520"/>
+        <c:axId val="150579840"/>
+        <c:axId val="150581632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150873984"/>
+        <c:axId val="150579840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -447,7 +498,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="150875520"/>
+        <c:crossAx val="150581632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -455,7 +506,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150875520"/>
+        <c:axId val="150581632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,7 +535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150873984"/>
+        <c:crossAx val="150579840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -779,11 +830,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="150804736"/>
-        <c:axId val="150814720"/>
+        <c:axId val="150973440"/>
+        <c:axId val="150979328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150804736"/>
+        <c:axId val="150973440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -792,7 +843,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="150814720"/>
+        <c:crossAx val="150979328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -800,7 +851,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150814720"/>
+        <c:axId val="150979328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -829,7 +880,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150804736"/>
+        <c:crossAx val="150973440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1344,11 +1395,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="152090496"/>
-        <c:axId val="152092032"/>
+        <c:axId val="151083648"/>
+        <c:axId val="151093632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152090496"/>
+        <c:axId val="151083648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1357,7 +1408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152092032"/>
+        <c:crossAx val="151093632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1365,7 +1416,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152092032"/>
+        <c:axId val="151093632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1395,7 +1446,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152090496"/>
+        <c:crossAx val="151083648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1910,11 +1961,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="150992384"/>
-        <c:axId val="150993920"/>
+        <c:axId val="151162880"/>
+        <c:axId val="151164416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150992384"/>
+        <c:axId val="151162880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1923,7 +1974,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150993920"/>
+        <c:crossAx val="151164416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1931,7 +1982,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150993920"/>
+        <c:axId val="151164416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1961,7 +2012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150992384"/>
+        <c:crossAx val="151162880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2694,11 +2745,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="157311744"/>
-        <c:axId val="157313280"/>
+        <c:axId val="151456000"/>
+        <c:axId val="151465984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="157311744"/>
+        <c:axId val="151456000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2707,7 +2758,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="157313280"/>
+        <c:crossAx val="151465984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2715,7 +2766,333 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="157313280"/>
+        <c:axId val="151465984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Coverage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151456000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.9999902626677827E-2"/>
+          <c:y val="0.8380946959768234"/>
+          <c:w val="0.89999987016890381"/>
+          <c:h val="8.6115838070366227E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="800">
+          <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>bc_policies!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unrestricted Dropping</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>bc_policies!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>perlbench</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bzip2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mcf</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gobmk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>hmmer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>sjeng</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h264ref</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>bc_policies!$B$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.91379999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53779999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75449999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96160000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.58260000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9819</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.78669999999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>bc_policies!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Source-Only Dropping</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>bc_policies!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>perlbench</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bzip2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mcf</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gobmk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>hmmer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>sjeng</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h264ref</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>bc_policies!$B$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.91190000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81569999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.73550000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99739999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99990000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99680000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="152659456"/>
+        <c:axId val="152660992"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="152659456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152660992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="152660992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2746,7 +3123,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="157311744"/>
+        <c:crossAx val="152659456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2757,9 +3134,966 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.9999902626677827E-2"/>
-          <c:y val="0.8380946959768234"/>
-          <c:w val="0.89999987016890381"/>
+          <c:x val="0.15034765521794421"/>
+          <c:y val="0.82643477813792954"/>
+          <c:w val="0.70754863959731584"/>
+          <c:h val="8.6115838070366227E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="800">
+          <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>bc_policies!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unrestricted Dropping</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>bc_policies!$B$5:$J$5</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>perlbench</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bzip2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mcf</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gobmk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>hmmer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>sjeng</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h264ref</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>bc_policies!$B$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9.6000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.7899999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.38080000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.3199999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.44119999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.46989999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.0000000000000001E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>bc_policies!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Source-Only Dropping</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>bc_policies!$B$5:$J$5</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>perlbench</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bzip2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mcf</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gobmk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>hmmer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>sjeng</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h264ref</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>bc_policies!$B$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.2697</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1905999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.8499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.29210000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1740999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.1409</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.44119999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.18479999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.10340000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="152586880"/>
+        <c:axId val="152617344"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="152586880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="152617344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="152617344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.60000000000000009"/>
+          <c:min val="-0.60000000000000009"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Overhead Difference</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152586880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14622551791247176"/>
+          <c:y val="0.84392465489627033"/>
+          <c:w val="0.70754863959731584"/>
+          <c:h val="8.6115838070366227E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="800">
+          <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>umc_policies!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unrestricted Dropping</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>umc_policies!$B$5:$J$5</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>perlbench</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bzip2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mcf</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gobmk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>hmmer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>sjeng</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h264ref</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>umc_policies!$B$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.15E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.6600000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.8999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.10630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.09E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.18629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8.2799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.5999999999999992E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>umc_policies!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Source-Only Dropping</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>umc_policies!$B$5:$J$5</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>perlbench</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bzip2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mcf</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gobmk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>hmmer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>sjeng</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h264ref</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>umc_policies!$B$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.1900000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.2499999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.0699999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.10630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.0800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.1000000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.186</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8.6499999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.7000000000000003E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="152839296"/>
+        <c:axId val="152840832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="152839296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="152840832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="152840832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Overhead Difference</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152839296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14622551791247176"/>
+          <c:y val="0.83226473705737647"/>
+          <c:w val="0.70754863959731584"/>
+          <c:h val="8.6115838070366227E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="800">
+          <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>umc_policies!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unrestricted Dropping</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>umc_policies!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>perlbench</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bzip2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mcf</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gobmk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>hmmer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>sjeng</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h264ref</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>umc_policies!$B$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.91379999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53779999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75449999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96160000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.58260000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9819</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.78669999999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>umc_policies!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Source-Only Dropping</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>umc_policies!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>perlbench</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bzip2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>mcf</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gobmk</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>hmmer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>sjeng</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>libquantum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h264ref</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>umc_policies!$B$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.91190000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81569999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.73550000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99739999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99990000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99680000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="152891392"/>
+        <c:axId val="152892928"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="152891392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152892928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="152892928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Coverage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152891392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14622551791247176"/>
+          <c:y val="0.84392465489627033"/>
+          <c:w val="0.70754863959731584"/>
           <c:h val="8.6115838070366227E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2842,10 +4176,58 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="324" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="324" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="347" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="347" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="324" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="324" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </chartsheet>
 </file>
@@ -2959,6 +4341,114 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="3080926" cy="2178403"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="2928869" cy="2028523"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="2928869" cy="2028523"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="3080926" cy="2178403"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -4655,6 +6145,1114 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride6.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="1F497D"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="EEECE1"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4F81BD"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="C0504D"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="9BBB59"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="8064A2"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4BACC6"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="F79646"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0000FF"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="800080"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="100000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride7.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="1F497D"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="EEECE1"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4F81BD"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="C0504D"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="9BBB59"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="8064A2"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4BACC6"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="F79646"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0000FF"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="800080"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="100000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride8.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="1F497D"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="EEECE1"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4F81BD"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="C0504D"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="9BBB59"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="8064A2"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4BACC6"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="F79646"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0000FF"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="800080"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="100000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride9.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="1F497D"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="EEECE1"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4F81BD"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="C0504D"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="9BBB59"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="8064A2"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4BACC6"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="F79646"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0000FF"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="800080"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="100000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:shade val="100000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
@@ -5457,12 +8055,258 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.91379999999999995</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.53779999999999994</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.75449999999999995</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.96160000000000001</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.58260000000000001</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.9819</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.78669999999999995</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.91190000000000004</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.81569999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.73550000000000004</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.99739999999999995</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.99680000000000002</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.81559999999999999</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-9.6000000000000002E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>-1.7899999999999999E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-0.38080000000000003</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-5.3199999999999997E-2</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>-0.44119999999999998</v>
+      </c>
+      <c r="I6" s="3">
+        <v>-0.46989999999999998</v>
+      </c>
+      <c r="J6" s="3">
+        <v>-5.0000000000000001E-4</v>
+      </c>
+      <c r="K6" s="3">
+        <v>-0.16</v>
+      </c>
+      <c r="L6" s="1">
+        <v>-0.47</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.2697</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4.1905999999999999</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-1.8499999999999999E-2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-0.29210000000000003</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.1740999999999999</v>
+      </c>
+      <c r="G7" s="3">
+        <v>15.1409</v>
+      </c>
+      <c r="H7" s="3">
+        <v>-0.44119999999999998</v>
+      </c>
+      <c r="I7" s="3">
+        <v>-0.18479999999999999</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.10340000000000001</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="L7" s="1">
+        <v>-0.44</v>
+      </c>
+      <c r="M7" s="1">
+        <v>15.14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5470,4 +8314,274 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.91379999999999995</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.53779999999999994</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.75449999999999995</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.96160000000000001</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.58260000000000001</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.9819</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.78669999999999995</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.91190000000000004</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.81569999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.73550000000000004</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.99739999999999995</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.99680000000000002</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.81559999999999999</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.15E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-6.6600000000000006E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-6.8999999999999999E-3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-0.10630000000000001</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-1.09E-2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>-0.18629999999999999</v>
+      </c>
+      <c r="I6" s="1">
+        <v>-8.2799999999999999E-2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="K6" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="L6" s="1">
+        <v>-0.19</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-7.2499999999999995E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-1.0699999999999999E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-0.10630000000000001</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-1.0800000000000001E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-4.1000000000000003E-3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>-0.186</v>
+      </c>
+      <c r="I7" s="1">
+        <v>-8.6499999999999994E-2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="K7" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="L7" s="1">
+        <v>-0.19</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>